<commit_message>
added batch to survival script
</commit_message>
<xml_diff>
--- a/data/rna-dna/sample_metadata.xlsx
+++ b/data/rna-dna/sample_metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/polyIC-larvae/data/rna-dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECF81DD-7A9C-DB4A-BABD-7D98017F7B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3D8C3A-6F22-DF43-8D09-2A53F46463F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34280" yWindow="-1460" windowWidth="27140" windowHeight="17500" xr2:uid="{0DAF8851-3CE0-B641-BA5A-C7AC4208D2FB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0DAF8851-3CE0-B641-BA5A-C7AC4208D2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="38">
   <si>
     <t>tube</t>
   </si>
@@ -91,17 +91,84 @@
   <si>
     <t xml:space="preserve">seed </t>
   </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Lifestage</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Treated</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>Larvae</t>
+  </si>
+  <si>
+    <t>Replicate-Tanks-per-Treatment</t>
+  </si>
+  <si>
+    <t>Total-Samples</t>
+  </si>
+  <si>
+    <t>8 days</t>
+  </si>
+  <si>
+    <t>n=2-3</t>
+  </si>
+  <si>
+    <t>n=1</t>
+  </si>
+  <si>
+    <t>14 days</t>
+  </si>
+  <si>
+    <t>Spat</t>
+  </si>
+  <si>
+    <t>60 days</t>
+  </si>
+  <si>
+    <t>n=3</t>
+  </si>
+  <si>
+    <t>135 days</t>
+  </si>
+  <si>
+    <t>n=2</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -125,8 +192,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,11 +529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD65DDB-7482-D846-9B42-22485EDC3B2E}">
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:O161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F161" sqref="F161"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,9 +541,11 @@
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -521,7 +591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,7 +614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -564,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -584,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -604,7 +674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -623,8 +693,23 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -643,8 +728,23 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -663,8 +763,23 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -683,8 +798,23 @@
       <c r="F10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -703,8 +833,23 @@
       <c r="F11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -723,8 +868,23 @@
       <c r="F12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -743,8 +903,23 @@
       <c r="F13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -763,8 +938,23 @@
       <c r="F14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -783,8 +973,23 @@
       <c r="F15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -803,8 +1008,23 @@
       <c r="F16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -826,8 +1046,23 @@
       <c r="G17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -849,8 +1084,15 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18">
+        <f>SUM(O8:O17)</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -870,7 +1112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -890,7 +1132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -910,7 +1152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -930,7 +1172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -950,7 +1192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -970,7 +1212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -990,7 +1232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1010,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1030,7 +1272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1050,7 +1292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1070,7 +1312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1090,7 +1332,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1110,7 +1352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>